<commit_message>
Added logic to clear existing summary sheets when necessary.
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evanm\Desktop\champstand\pyChampstandings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC4FB01-1F8D-45B8-8ACA-234BFF4F6D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4AF672-3B50-413B-A34C-EB5898B19010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24825" yWindow="2805" windowWidth="19080" windowHeight="15120" activeTab="1" xr2:uid="{B53C6510-5989-45F7-B0AE-7D0C63CD7255}"/>
+    <workbookView xWindow="-28920" yWindow="2445" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B53C6510-5989-45F7-B0AE-7D0C63CD7255}"/>
   </bookViews>
   <sheets>
     <sheet name="rawdata_Clio" sheetId="1" r:id="rId1"/>
     <sheet name="rawdata_F3" sheetId="2" r:id="rId2"/>
+    <sheet name="summary_F3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
   <si>
     <t>Week</t>
   </si>
@@ -61,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ray </t>
+  </si>
+  <si>
+    <t>sdfds</t>
   </si>
 </sst>
 </file>
@@ -516,7 +520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8E1C86-FA81-41CB-8903-8A97ABAC4786}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -606,4 +610,22 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7CA3EE-5588-4CFC-94B6-0BA76074BF59}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Started implementing the "Business logic." Read in all results and start calculating points and sorting drivers according to results.
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evanm\Desktop\champstand\pyChampstandings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4AF672-3B50-413B-A34C-EB5898B19010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056CE3AE-F73D-4B81-ADD4-1D6E34620B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2445" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B53C6510-5989-45F7-B0AE-7D0C63CD7255}"/>
+    <workbookView xWindow="-28920" yWindow="2445" windowWidth="29040" windowHeight="15840" xr2:uid="{B53C6510-5989-45F7-B0AE-7D0C63CD7255}"/>
   </bookViews>
   <sheets>
     <sheet name="rawdata_Clio" sheetId="1" r:id="rId1"/>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A581DB-E75B-4759-9137-2FBB50F3C45C}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,6 +508,29 @@
       </c>
       <c r="H3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -616,7 +639,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7CA3EE-5588-4CFC-94B6-0BA76074BF59}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Automatically run through main business logic and generate results ready to print. Fixed some issues with sorting logic and added output strings.
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evanm\Desktop\champstand\pyChampstandings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056CE3AE-F73D-4B81-ADD4-1D6E34620B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDADB5B-D78E-431C-9178-D12B6CEEFD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2445" windowWidth="29040" windowHeight="15840" xr2:uid="{B53C6510-5989-45F7-B0AE-7D0C63CD7255}"/>
+    <workbookView xWindow="19470" yWindow="2610" windowWidth="19080" windowHeight="15120" activeTab="1" xr2:uid="{B53C6510-5989-45F7-B0AE-7D0C63CD7255}"/>
   </bookViews>
   <sheets>
     <sheet name="rawdata_Clio" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
   <si>
     <t>Week</t>
   </si>
@@ -419,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A581DB-E75B-4759-9137-2FBB50F3C45C}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,23 +514,26 @@
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" s="1">
+        <v>44695</v>
+      </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -541,10 +544,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8E1C86-FA81-41CB-8903-8A97ABAC4786}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,6 +630,32 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44696</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add the ability to custom designate output file.
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,41 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evanm\Desktop\champstand\pyChampstandings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDADB5B-D78E-431C-9178-D12B6CEEFD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54B0047-0238-4D1E-9018-0DF49D0FAD7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19470" yWindow="2610" windowWidth="19080" windowHeight="15120" activeTab="1" xr2:uid="{B53C6510-5989-45F7-B0AE-7D0C63CD7255}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{B53C6510-5989-45F7-B0AE-7D0C63CD7255}"/>
   </bookViews>
   <sheets>
-    <sheet name="rawdata_Clio" sheetId="1" r:id="rId1"/>
-    <sheet name="rawdata_F3" sheetId="2" r:id="rId2"/>
-    <sheet name="summary_F3" sheetId="3" r:id="rId3"/>
+    <sheet name="rawdata_Alpine" sheetId="1" r:id="rId1"/>
+    <sheet name="rawdata_GP" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t>Week</t>
   </si>
@@ -49,22 +40,13 @@
     <t>Mike</t>
   </si>
   <si>
-    <t>Zach</t>
-  </si>
-  <si>
-    <t>DNP</t>
-  </si>
-  <si>
-    <t>Steve</t>
-  </si>
-  <si>
     <t>Driver</t>
   </si>
   <si>
     <t xml:space="preserve">Ray </t>
   </si>
   <si>
-    <t>sdfds</t>
+    <t>DNS</t>
   </si>
 </sst>
 </file>
@@ -417,9 +399,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A581DB-E75B-4759-9137-2FBB50F3C45C}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -432,12 +414,12 @@
     <col min="20" max="20" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -449,27 +431,21 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>44680</v>
+        <v>45010</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -477,64 +453,58 @@
       <c r="F2">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>44688</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
+        <v>45017</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>44695</v>
+        <v>45024</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>5</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -544,10 +514,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8E1C86-FA81-41CB-8903-8A97ABAC4786}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,12 +525,12 @@
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -572,21 +542,15 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>44680</v>
+        <v>45010</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -600,45 +564,33 @@
       <c r="F2">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>44688</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
+        <v>45017</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>44696</v>
+        <v>45024</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -649,35 +601,21 @@
       <c r="E4">
         <v>3</v>
       </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7CA3EE-5588-4CFC-94B6-0BA76074BF59}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>